<commit_message>
Add statistics from April 13
</commit_message>
<xml_diff>
--- a/Folkhalsomyndigheten_Covid19.xlsx
+++ b/Folkhalsomyndigheten_Covid19.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dfs-srv1.fohm.local\common\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19695" windowHeight="10455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 12 Apr 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 13 Apr 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Statistikdatum</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Data uppdateras dagligen kl 11.30 och finns tillgägliga dagligen kl 14.00. Läs mer på https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/aktuellt-epidemiologiskt-lage/</t>
-  </si>
-  <si>
-    <t>uppgift saknas</t>
   </si>
 </sst>
 </file>
@@ -508,16 +505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -4500,7 +4494,7 @@
         <v>43920</v>
       </c>
       <c r="B57" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -4536,7 +4530,7 @@
         <v>5</v>
       </c>
       <c r="N57" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O57" s="2">
         <v>60</v>
@@ -5210,7 +5204,7 @@
         <v>43930</v>
       </c>
       <c r="B67" s="2">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="C67" s="2">
         <v>1</v>
@@ -5270,7 +5264,7 @@
         <v>117</v>
       </c>
       <c r="V67" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="W67" s="2">
         <v>54</v>
@@ -5281,7 +5275,7 @@
         <v>43931</v>
       </c>
       <c r="B68" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C68" s="2">
         <v>1</v>
@@ -5317,7 +5311,7 @@
         <v>24</v>
       </c>
       <c r="N68" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O68" s="2">
         <v>41</v>
@@ -5352,13 +5346,13 @@
         <v>43932</v>
       </c>
       <c r="B69" s="2">
-        <v>330</v>
+        <v>389</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
       </c>
       <c r="D69" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -5373,7 +5367,7 @@
         <v>2</v>
       </c>
       <c r="I69" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J69" s="2">
         <v>3</v>
@@ -5382,19 +5376,19 @@
         <v>10</v>
       </c>
       <c r="L69" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M69" s="2">
         <v>6</v>
       </c>
       <c r="N69" s="2">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="O69" s="2">
         <v>22</v>
       </c>
       <c r="P69" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q69" s="2">
         <v>2</v>
@@ -5406,10 +5400,10 @@
         <v>0</v>
       </c>
       <c r="T69" s="2">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="U69" s="2">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="V69" s="2">
         <v>8</v>
@@ -5423,69 +5417,140 @@
         <v>43933</v>
       </c>
       <c r="B70" s="2">
-        <v>99</v>
+        <v>419</v>
       </c>
       <c r="C70" s="2">
         <v>0</v>
       </c>
       <c r="D70" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
       </c>
       <c r="F70" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G70" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H70" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I70" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J70" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L70" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M70" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N70" s="2">
+        <v>174</v>
+      </c>
+      <c r="O70" s="2">
+        <v>7</v>
+      </c>
+      <c r="P70" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>2</v>
+      </c>
+      <c r="R70" s="2">
+        <v>0</v>
+      </c>
+      <c r="S70" s="2">
+        <v>5</v>
+      </c>
+      <c r="T70" s="2">
+        <v>15</v>
+      </c>
+      <c r="U70" s="2">
+        <v>43</v>
+      </c>
+      <c r="V70" s="2">
+        <v>64</v>
+      </c>
+      <c r="W70" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
+      <c r="A71" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B71" s="2">
         <v>83</v>
       </c>
-      <c r="O70" s="2">
-        <v>0</v>
-      </c>
-      <c r="P70" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q70" s="2">
-        <v>0</v>
-      </c>
-      <c r="R70" s="2">
-        <v>0</v>
-      </c>
-      <c r="S70" s="2">
-        <v>0</v>
-      </c>
-      <c r="T70" s="2">
-        <v>0</v>
-      </c>
-      <c r="U70" s="2">
-        <v>14</v>
-      </c>
-      <c r="V70" s="2">
-        <v>0</v>
-      </c>
-      <c r="W70" s="2">
+      <c r="C71" s="2">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0</v>
+      </c>
+      <c r="G71" s="2">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0</v>
+      </c>
+      <c r="J71" s="2">
+        <v>0</v>
+      </c>
+      <c r="K71" s="2">
+        <v>0</v>
+      </c>
+      <c r="L71" s="2">
+        <v>0</v>
+      </c>
+      <c r="M71" s="2">
+        <v>0</v>
+      </c>
+      <c r="N71" s="2">
+        <v>74</v>
+      </c>
+      <c r="O71" s="2">
+        <v>0</v>
+      </c>
+      <c r="P71" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>0</v>
+      </c>
+      <c r="R71" s="2">
+        <v>0</v>
+      </c>
+      <c r="S71" s="2">
+        <v>0</v>
+      </c>
+      <c r="T71" s="2">
+        <v>0</v>
+      </c>
+      <c r="U71" s="2">
+        <v>9</v>
+      </c>
+      <c r="V71" s="2">
+        <v>0</v>
+      </c>
+      <c r="W71" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5496,16 +5561,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5752,7 +5814,7 @@
         <v>43930</v>
       </c>
       <c r="B31" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5760,7 +5822,7 @@
         <v>43931</v>
       </c>
       <c r="B32" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -5768,7 +5830,7 @@
         <v>43932</v>
       </c>
       <c r="B33" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5776,14 +5838,22 @@
         <v>43933</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>50</v>
+      <c r="A35" s="1">
+        <v>43934</v>
       </c>
       <c r="B35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
         <v>13</v>
       </c>
     </row>
@@ -5794,7 +5864,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -6015,7 +6085,7 @@
         <v>43921</v>
       </c>
       <c r="B27" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -6023,7 +6093,7 @@
         <v>43922</v>
       </c>
       <c r="B28" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -6055,7 +6125,7 @@
         <v>43926</v>
       </c>
       <c r="B32" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -6063,7 +6133,7 @@
         <v>43927</v>
       </c>
       <c r="B33" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -6103,7 +6173,7 @@
         <v>43932</v>
       </c>
       <c r="B38" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -6111,7 +6181,15 @@
         <v>43933</v>
       </c>
       <c r="B39" s="2">
-        <v>1</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B40" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6157,7 +6235,7 @@
         <v>25.688257217407227</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -6168,13 +6246,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="C3" s="2">
-        <v>109.73517608642578</v>
+        <v>119.80580902099609</v>
       </c>
       <c r="D3" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>37</v>
@@ -6202,13 +6280,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="C5" s="2">
-        <v>94.995513916015625</v>
+        <v>100.91098022460938</v>
       </c>
       <c r="D5" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
         <v>27</v>
@@ -6219,10 +6297,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C6" s="2">
-        <v>54.515827178955078</v>
+        <v>55.414440155029297</v>
       </c>
       <c r="D6" s="2">
         <v>14</v>
@@ -6236,10 +6314,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C7" s="2">
-        <v>97.087379455566406</v>
+        <v>100.14524841308594</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
@@ -6253,13 +6331,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="C8" s="2">
-        <v>93.509605407714844</v>
+        <v>96.2598876953125</v>
       </c>
       <c r="D8" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2">
         <v>25</v>
@@ -6270,13 +6348,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2">
-        <v>27.704668045043945</v>
+        <v>28.519512176513672</v>
       </c>
       <c r="D9" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
         <v>4</v>
@@ -6287,10 +6365,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C10" s="2">
-        <v>48.146366119384766</v>
+        <v>48.642719268798828</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -6304,13 +6382,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C11" s="2">
-        <v>53.580066680908203</v>
+        <v>54.779621124267578</v>
       </c>
       <c r="D11" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2">
         <v>7</v>
@@ -6321,16 +6399,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="C12" s="2">
-        <v>31.571453094482422</v>
+        <v>32.587547302246094</v>
       </c>
       <c r="D12" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -6338,16 +6416,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>4397</v>
+        <v>4575</v>
       </c>
       <c r="C13" s="2">
-        <v>184.97476196289063</v>
+        <v>192.46293640136719</v>
       </c>
       <c r="D13" s="2">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E13" s="2">
-        <v>528</v>
+        <v>543</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6355,13 +6433,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="C14" s="2">
-        <v>222.15499877929688</v>
+        <v>224.50762939453125</v>
       </c>
       <c r="D14" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2">
         <v>83</v>
@@ -6372,13 +6450,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="C15" s="2">
-        <v>117.01454162597656</v>
+        <v>121.184326171875</v>
       </c>
       <c r="D15" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2">
         <v>30</v>
@@ -6389,10 +6467,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C16" s="2">
-        <v>26.556756973266602</v>
+        <v>27.264936447143555</v>
       </c>
       <c r="D16" s="2">
         <v>9</v>
@@ -6412,10 +6490,10 @@
         <v>67.344772338867188</v>
       </c>
       <c r="D17" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6423,13 +6501,13 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C18" s="2">
-        <v>40.758598327636719</v>
+        <v>42.796527862548828</v>
       </c>
       <c r="D18" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="2">
         <v>8</v>
@@ -6440,13 +6518,13 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>304</v>
+        <v>346</v>
       </c>
       <c r="C19" s="2">
-        <v>110.20681762695313</v>
+        <v>125.43276214599609</v>
       </c>
       <c r="D19" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2">
         <v>16</v>
@@ -6457,16 +6535,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>1018</v>
+        <v>1064</v>
       </c>
       <c r="C20" s="2">
-        <v>58.984367370605469</v>
+        <v>61.649673461914063</v>
       </c>
       <c r="D20" s="2">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E20" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -6474,13 +6552,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>316</v>
+        <v>383</v>
       </c>
       <c r="C21" s="2">
-        <v>103.67283630371094</v>
+        <v>125.65410614013672</v>
       </c>
       <c r="D21" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
@@ -6491,10 +6569,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>951</v>
+        <v>970</v>
       </c>
       <c r="C22" s="2">
-        <v>204.29864501953125</v>
+        <v>208.38032531738281</v>
       </c>
       <c r="D22" s="2">
         <v>45</v>
@@ -6512,9 +6590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -6537,13 +6613,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>5131</v>
+        <v>5350</v>
       </c>
       <c r="C2" s="2">
-        <v>633</v>
+        <v>648</v>
       </c>
       <c r="D2" s="2">
-        <v>523</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6551,13 +6627,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>5350</v>
+        <v>5596</v>
       </c>
       <c r="C3" s="2">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D3" s="2">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6583,7 +6659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -6606,7 +6684,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -6620,7 +6698,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -6634,10 +6712,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>767</v>
+        <v>802</v>
       </c>
       <c r="C4" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -6648,7 +6726,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>978</v>
+        <v>1025</v>
       </c>
       <c r="C5" s="2">
         <v>39</v>
@@ -6662,10 +6740,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>1342</v>
+        <v>1400</v>
       </c>
       <c r="C6" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
@@ -6676,13 +6754,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>1813</v>
+        <v>1900</v>
       </c>
       <c r="C7" s="2">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D7" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6690,13 +6768,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>1460</v>
+        <v>1529</v>
       </c>
       <c r="C8" s="2">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D8" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6704,13 +6782,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>1475</v>
+        <v>1541</v>
       </c>
       <c r="C9" s="2">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D9" s="2">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6718,13 +6796,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>1599</v>
+        <v>1672</v>
       </c>
       <c r="C10" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6732,13 +6810,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>819</v>
+        <v>848</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6746,7 +6824,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>

</xml_diff>